<commit_message>
EPBDS-10059 Minor Demo examples update
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/DEMO/org.openl.rules.demo/data/openl-demo/design-repository/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
+++ b/DEMO/org.openl.rules.demo/data/openl-demo/design-repository/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\OpenL\draft docs for mercurial\tut and examples with logo\org.openl.rules.demo.tutorials\Tutorial 1 - Introduction to Decision Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\openl-demo-app-5.23.3\apache-tomcat-9.0.30\openl-demo\user-workspace\DEFAULT\Tutorial 1 - Introduction to Decision Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0641ECB-E5EA-474E-B0FA-E7F99B027232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -34,13 +35,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stanislav Shor</author>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="D25" authorId="0" shapeId="0">
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="1" shapeId="0">
+    <comment ref="D26" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="1" shapeId="0">
+    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -211,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="1" shapeId="0">
+    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -226,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D59" authorId="1" shapeId="0">
+    <comment ref="D59" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F59" authorId="1" shapeId="0">
+    <comment ref="F59" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -255,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D60" authorId="1" shapeId="0">
+    <comment ref="D60" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -269,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F60" authorId="1" shapeId="0">
+    <comment ref="F60" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -283,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E66" authorId="1" shapeId="0">
+    <comment ref="E66" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -297,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C71" authorId="1" shapeId="0">
+    <comment ref="C71" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -311,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D75" authorId="1" shapeId="0">
+    <comment ref="D75" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -330,12 +331,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="D25" authorId="0" shapeId="0">
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -349,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="0" shapeId="0">
+    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -363,7 +364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E28" authorId="0" shapeId="0">
+    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -377,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -391,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -405,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0" shapeId="0">
+    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -424,12 +425,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -443,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E81" authorId="0" shapeId="0">
+    <comment ref="E81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -457,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E108" authorId="0" shapeId="0">
+    <comment ref="E108" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1099,31 +1100,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">SimpleLookup DoubleValue </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>CarPrice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (String country, String carBrand, String carModel)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Rules String </t>
     </r>
     <r>
@@ -1344,81 +1320,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>DriverPremium1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>DriverPremium2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleLookup DoubleValue </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>DriverPremium5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverdriverMaritalStatus)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">            A </t>
     </r>
     <r>
@@ -1616,8 +1517,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">SimpleRules DoubleValue </t>
+    <t>Country</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double </t>
     </r>
     <r>
       <rPr>
@@ -1627,7 +1531,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium3</t>
+      <t>DriverPremium1</t>
     </r>
     <r>
       <rPr>
@@ -1642,7 +1546,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
+      <t xml:space="preserve">Rules Double </t>
     </r>
     <r>
       <rPr>
@@ -1652,7 +1556,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium4</t>
+      <t>DriverPremium2</t>
     </r>
     <r>
       <rPr>
@@ -1666,17 +1570,114 @@
     </r>
   </si>
   <si>
-    <t>Country</t>
+    <r>
+      <t xml:space="preserve">SimpleRules Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>DriverPremium3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>DriverPremium4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleLookup Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>DriverPremium5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverdriverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleLookup Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>CarPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String country, String carBrand, String carModel)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
-    <numFmt numFmtId="166" formatCode="\ &quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="\ &quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2274,25 +2275,25 @@
     <xf numFmtId="3" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2304,16 +2305,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -2340,7 +2341,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2352,34 +2353,34 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2391,16 +2392,16 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2474,16 +2475,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2505,7 +2506,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 5" xfId="2"/>
+    <cellStyle name="Обычный 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2545,7 +2546,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2618,7 +2625,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 1"/>
+        <xdr:cNvPr id="3" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2669,7 +2682,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 1"/>
+        <xdr:cNvPr id="2" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3074,20 +3093,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9.140625" style="3" collapsed="1"/>
-    <col min="10" max="10" width="19.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="9" width="9.109375" style="3" collapsed="1"/>
+    <col min="10" max="10" width="19.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="70" t="s">
         <v>17</v>
       </c>
@@ -3099,14 +3118,14 @@
       <c r="H3" s="70"/>
       <c r="I3" s="70"/>
     </row>
-    <row r="4" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
       <c r="G4" s="43"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3118,7 +3137,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3130,7 +3149,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="73" t="s">
         <v>18</v>
@@ -3144,7 +3163,7 @@
       <c r="J8" s="74"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="75"/>
       <c r="D9" s="75"/>
@@ -3156,7 +3175,7 @@
       <c r="J9" s="75"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="75"/>
       <c r="D10" s="75"/>
@@ -3168,7 +3187,7 @@
       <c r="J10" s="75"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="75"/>
       <c r="D11" s="75"/>
@@ -3180,7 +3199,7 @@
       <c r="J11" s="75"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="75"/>
       <c r="D12" s="75"/>
@@ -3192,7 +3211,7 @@
       <c r="J12" s="75"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="75"/>
       <c r="D13" s="75"/>
@@ -3204,7 +3223,7 @@
       <c r="J13" s="75"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="75"/>
       <c r="D14" s="75"/>
@@ -3216,7 +3235,7 @@
       <c r="J14" s="75"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="75"/>
       <c r="D15" s="75"/>
@@ -3228,7 +3247,7 @@
       <c r="J15" s="75"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -3240,7 +3259,7 @@
       <c r="J16" s="75"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="75"/>
       <c r="D17" s="75"/>
@@ -3252,7 +3271,7 @@
       <c r="J17" s="75"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
       <c r="C18" s="75"/>
       <c r="D18" s="75"/>
@@ -3264,7 +3283,7 @@
       <c r="J18" s="75"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="75"/>
       <c r="D19" s="75"/>
@@ -3276,7 +3295,7 @@
       <c r="J19" s="75"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="75"/>
       <c r="D20" s="75"/>
@@ -3288,7 +3307,7 @@
       <c r="J20" s="75"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="75"/>
       <c r="D21" s="75"/>
@@ -3300,7 +3319,7 @@
       <c r="J21" s="75"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="76"/>
       <c r="D22" s="76"/>
@@ -3312,7 +3331,7 @@
       <c r="J22" s="76"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3324,7 +3343,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3336,7 +3355,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3348,7 +3367,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -3360,7 +3379,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -3372,7 +3391,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="77" t="s">
         <v>33</v>
@@ -3386,7 +3405,7 @@
       <c r="J28" s="77"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
       <c r="C29" s="71" t="s">
         <v>89</v>
@@ -3400,7 +3419,7 @@
       <c r="J29" s="71"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="71" t="s">
         <v>91</v>
@@ -3414,7 +3433,7 @@
       <c r="J30" s="71"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="71" t="s">
         <v>92</v>
@@ -3428,7 +3447,7 @@
       <c r="J31" s="71"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="71" t="s">
         <v>93</v>
@@ -3442,7 +3461,7 @@
       <c r="J32" s="71"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="71" t="s">
         <v>94</v>
@@ -3456,7 +3475,7 @@
       <c r="J33" s="71"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="71" t="s">
         <v>95</v>
@@ -3470,7 +3489,7 @@
       <c r="J34" s="71"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="C35" s="71" t="s">
         <v>96</v>
@@ -3484,7 +3503,7 @@
       <c r="J35" s="71"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="71" t="s">
         <v>97</v>
@@ -3498,7 +3517,7 @@
       <c r="J36" s="71"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="72" t="s">
         <v>98</v>
@@ -3512,7 +3531,7 @@
       <c r="J37" s="72"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -3524,7 +3543,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -3536,7 +3555,7 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -3565,16 +3584,16 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C28:J28" location="_st1" display="Step1. Decision Table and its structure"/>
-    <hyperlink ref="C30:J30" location="_st2" display=" Step2. Lookup Table and its structure"/>
-    <hyperlink ref="C31:J31" location="_st21" display="     Step2-1. Simple Lookup Table"/>
-    <hyperlink ref="C32:J32" location="_st22" display="     Step2-2. Lookup Table with several horizontal conditions"/>
-    <hyperlink ref="C29:J29" location="_st11" display="     Step1-1. Simple Decision Table"/>
-    <hyperlink ref="C33:J33" location="_st3" display=" Step3. Examples of Decision Tables"/>
-    <hyperlink ref="C34:J34" location="_st31" display="     Step3-1. Demonstrating transposed Decision Table"/>
-    <hyperlink ref="C35:J35" location="_st32" display="     Step3-2. Demonstrating usage of 2 parameters for one condition"/>
-    <hyperlink ref="C36:J36" location="_st33" display="     Step3-3. Demonstrating usage of Ranges in Decision Tables"/>
-    <hyperlink ref="C37:J37" location="_st34" display="     Step3-4. Demonstrating Actions in Decision Tables"/>
+    <hyperlink ref="C28:J28" location="_st1" display="Step1. Decision Table and its structure" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C30:J30" location="_st2" display=" Step2. Lookup Table and its structure" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C31:J31" location="_st21" display="     Step2-1. Simple Lookup Table" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C32:J32" location="_st22" display="     Step2-2. Lookup Table with several horizontal conditions" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C29:J29" location="_st11" display="     Step1-1. Simple Decision Table" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C33:J33" location="_st3" display=" Step3. Examples of Decision Tables" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C34:J34" location="_st31" display="     Step3-1. Demonstrating transposed Decision Table" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C35:J35" location="_st32" display="     Step3-2. Demonstrating usage of 2 parameters for one condition" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C36:J36" location="_st33" display="     Step3-3. Demonstrating usage of Ranges in Decision Tables" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C37:J37" location="_st34" display="     Step3-4. Demonstrating Actions in Decision Tables" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3584,26 +3603,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105:F105"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" style="1" collapsed="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="19.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" s="3" customFormat="1" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="78" t="s">
         <v>88</v>
       </c>
@@ -3612,15 +3633,15 @@
       <c r="E3" s="78"/>
       <c r="F3" s="78"/>
     </row>
-    <row r="4" spans="2:7" s="3" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" s="3" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3628,7 +3649,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="2:7" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" s="3" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3636,7 +3657,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="80" t="s">
         <v>33</v>
@@ -3646,7 +3667,7 @@
       <c r="F8" s="80"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:7" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" s="3" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -3654,7 +3675,7 @@
       <c r="F9" s="81"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="66"/>
@@ -3662,7 +3683,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -3670,17 +3691,17 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="84" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
       <c r="F12" s="84"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -3688,7 +3709,7 @@
       <c r="F13" s="85"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="85"/>
       <c r="D14" s="85"/>
@@ -3696,7 +3717,7 @@
       <c r="F14" s="85"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B15" s="9"/>
       <c r="C15" s="85"/>
       <c r="D15" s="85"/>
@@ -3704,7 +3725,7 @@
       <c r="F15" s="85"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="85"/>
       <c r="D16" s="85"/>
@@ -3712,7 +3733,7 @@
       <c r="F16" s="85"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="85"/>
       <c r="D17" s="85"/>
@@ -3720,7 +3741,7 @@
       <c r="F17" s="85"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
       <c r="C18" s="85"/>
       <c r="D18" s="85"/>
@@ -3728,7 +3749,7 @@
       <c r="F18" s="85"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="C19" s="85"/>
       <c r="D19" s="85"/>
@@ -3736,7 +3757,7 @@
       <c r="F19" s="85"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -3744,7 +3765,7 @@
       <c r="F20" s="85"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="85"/>
       <c r="D21" s="85"/>
@@ -3752,7 +3773,7 @@
       <c r="F21" s="85"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="2:7" s="3" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" s="3" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="86"/>
       <c r="D22" s="86"/>
@@ -3760,7 +3781,7 @@
       <c r="F22" s="86"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -3768,7 +3789,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -3776,17 +3797,17 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="2:7" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="79" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E25" s="79"/>
       <c r="F25" s="79"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="2:7" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
@@ -3800,7 +3821,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13" t="s">
@@ -3814,7 +3835,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13" t="s">
@@ -3828,7 +3849,7 @@
       </c>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="13" t="s">
@@ -3842,7 +3863,7 @@
       </c>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="2:7" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="15" t="s">
@@ -3856,7 +3877,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="2:7" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="16">
@@ -3870,7 +3891,7 @@
       </c>
       <c r="G31" s="12"/>
     </row>
-    <row r="32" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="17">
@@ -3884,7 +3905,7 @@
       </c>
       <c r="G32" s="12"/>
     </row>
-    <row r="33" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="17">
@@ -3898,7 +3919,7 @@
       </c>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="2:14" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="19">
@@ -3912,7 +3933,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="2:14" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -3920,7 +3941,7 @@
       <c r="F35" s="47"/>
       <c r="G35" s="12"/>
     </row>
-    <row r="36" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -3928,7 +3949,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="84" t="s">
         <v>34</v>
@@ -3938,7 +3959,7 @@
       <c r="F37" s="84"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B38" s="9"/>
       <c r="C38" s="85"/>
       <c r="D38" s="85"/>
@@ -3946,7 +3967,7 @@
       <c r="F38" s="85"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B39" s="9"/>
       <c r="C39" s="85"/>
       <c r="D39" s="85"/>
@@ -3954,7 +3975,7 @@
       <c r="F39" s="85"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B40" s="9"/>
       <c r="C40" s="85"/>
       <c r="D40" s="85"/>
@@ -3962,7 +3983,7 @@
       <c r="F40" s="85"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
       <c r="C41" s="85"/>
       <c r="D41" s="85"/>
@@ -3970,7 +3991,7 @@
       <c r="F41" s="85"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B42" s="9"/>
       <c r="C42" s="85"/>
       <c r="D42" s="85"/>
@@ -3978,7 +3999,7 @@
       <c r="F42" s="85"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
       <c r="C43" s="85"/>
       <c r="D43" s="85"/>
@@ -3986,7 +4007,7 @@
       <c r="F43" s="85"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B44" s="9"/>
       <c r="C44" s="85"/>
       <c r="D44" s="85"/>
@@ -3994,7 +4015,7 @@
       <c r="F44" s="85"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B45" s="9"/>
       <c r="C45" s="85"/>
       <c r="D45" s="85"/>
@@ -4002,7 +4023,7 @@
       <c r="F45" s="85"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="85"/>
       <c r="D46" s="85"/>
@@ -4010,7 +4031,7 @@
       <c r="F46" s="85"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="86"/>
       <c r="D47" s="86"/>
@@ -4021,7 +4042,7 @@
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
     </row>
-    <row r="48" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -4032,7 +4053,7 @@
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
     </row>
-    <row r="49" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -4040,7 +4061,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B50" s="9"/>
       <c r="C50" s="84" t="s">
         <v>45</v>
@@ -4050,7 +4071,7 @@
       <c r="F50" s="84"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B51" s="9"/>
       <c r="C51" s="85"/>
       <c r="D51" s="85"/>
@@ -4058,7 +4079,7 @@
       <c r="F51" s="85"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B52" s="9"/>
       <c r="C52" s="85"/>
       <c r="D52" s="85"/>
@@ -4066,7 +4087,7 @@
       <c r="F52" s="85"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B53" s="9"/>
       <c r="C53" s="85"/>
       <c r="D53" s="85"/>
@@ -4074,7 +4095,7 @@
       <c r="F53" s="85"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B54" s="9"/>
       <c r="C54" s="86"/>
       <c r="D54" s="86"/>
@@ -4082,7 +4103,7 @@
       <c r="F54" s="86"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -4090,7 +4111,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -4098,17 +4119,17 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="2:13" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="79" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E57" s="79"/>
       <c r="F57" s="79"/>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="13" t="s">
@@ -4122,19 +4143,19 @@
       </c>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="39" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="12"/>
     </row>
-    <row r="60" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="13" t="s">
@@ -4146,7 +4167,7 @@
       <c r="F60" s="13"/>
       <c r="G60" s="12"/>
     </row>
-    <row r="61" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="15" t="s">
@@ -4160,7 +4181,7 @@
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="2:13" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="16" t="s">
@@ -4174,7 +4195,7 @@
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="17" t="s">
@@ -4188,7 +4209,7 @@
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="17" t="s">
@@ -4203,7 +4224,7 @@
       <c r="G64" s="12"/>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="17" t="s">
@@ -4218,7 +4239,7 @@
       <c r="G65" s="12"/>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="21" t="s">
@@ -4231,7 +4252,7 @@
       <c r="G66" s="12"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="2:13" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -4239,7 +4260,7 @@
       <c r="F67" s="47"/>
       <c r="G67" s="12"/>
     </row>
-    <row r="68" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -4247,7 +4268,7 @@
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
     </row>
-    <row r="69" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -4255,17 +4276,17 @@
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
     </row>
-    <row r="70" spans="2:13" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="C70" s="79" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D70" s="79"/>
       <c r="E70" s="79"/>
       <c r="F70" s="79"/>
       <c r="G70" s="12"/>
     </row>
-    <row r="71" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
       <c r="C71" s="13" t="s">
         <v>0</v>
@@ -4281,19 +4302,19 @@
       </c>
       <c r="G71" s="12"/>
     </row>
-    <row r="72" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="12"/>
     </row>
-    <row r="73" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13" t="s">
@@ -4306,7 +4327,7 @@
       <c r="G73" s="12"/>
       <c r="L73" s="10"/>
     </row>
-    <row r="74" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
       <c r="C74" s="15" t="s">
         <v>32</v>
@@ -4323,7 +4344,7 @@
       <c r="G74" s="12"/>
       <c r="L74" s="8"/>
     </row>
-    <row r="75" spans="2:13" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="C75" s="22" t="s">
         <v>27</v>
@@ -4340,7 +4361,7 @@
       <c r="G75" s="12"/>
       <c r="L75" s="8"/>
     </row>
-    <row r="76" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="C76" s="24" t="s">
         <v>28</v>
@@ -4355,7 +4376,7 @@
       <c r="G76" s="12"/>
       <c r="L76" s="8"/>
     </row>
-    <row r="77" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
       <c r="C77" s="24" t="s">
         <v>29</v>
@@ -4372,7 +4393,7 @@
       <c r="G77" s="12"/>
       <c r="L77" s="8"/>
     </row>
-    <row r="78" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="C78" s="24" t="s">
         <v>30</v>
@@ -4387,7 +4408,7 @@
       <c r="G78" s="12"/>
       <c r="L78" s="8"/>
     </row>
-    <row r="79" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="12"/>
       <c r="C79" s="27" t="s">
         <v>31</v>
@@ -4401,7 +4422,7 @@
       </c>
       <c r="G79" s="12"/>
     </row>
-    <row r="80" spans="2:13" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -4409,7 +4430,7 @@
       <c r="F80" s="47"/>
       <c r="G80" s="12"/>
     </row>
-    <row r="81" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -4417,7 +4438,7 @@
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
     </row>
-    <row r="82" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -4425,7 +4446,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B83" s="9"/>
       <c r="C83" s="84" t="s">
         <v>84</v>
@@ -4435,7 +4456,7 @@
       <c r="F83" s="84"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B84" s="9"/>
       <c r="C84" s="86"/>
       <c r="D84" s="86"/>
@@ -4443,7 +4464,7 @@
       <c r="F84" s="86"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -4451,7 +4472,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -4459,7 +4480,7 @@
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
     </row>
-    <row r="87" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -4467,7 +4488,7 @@
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
     </row>
-    <row r="88" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -4475,7 +4496,7 @@
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
     </row>
-    <row r="89" spans="1:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -4483,7 +4504,7 @@
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
     </row>
-    <row r="90" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="12"/>
       <c r="C90" s="87" t="s">
@@ -4494,7 +4515,7 @@
       <c r="F90" s="87"/>
       <c r="G90" s="12"/>
     </row>
-    <row r="91" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B91" s="12"/>
       <c r="C91" s="67"/>
       <c r="D91" s="67"/>
@@ -4502,7 +4523,7 @@
       <c r="F91" s="67"/>
       <c r="G91" s="12"/>
     </row>
-    <row r="92" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -4510,7 +4531,7 @@
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
     </row>
-    <row r="93" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B93" s="12"/>
       <c r="C93" s="84" t="s">
         <v>49</v>
@@ -4520,7 +4541,7 @@
       <c r="F93" s="84"/>
       <c r="G93" s="12"/>
     </row>
-    <row r="94" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B94" s="12"/>
       <c r="C94" s="85"/>
       <c r="D94" s="85"/>
@@ -4528,7 +4549,7 @@
       <c r="F94" s="85"/>
       <c r="G94" s="12"/>
     </row>
-    <row r="95" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B95" s="12"/>
       <c r="C95" s="85"/>
       <c r="D95" s="85"/>
@@ -4536,7 +4557,7 @@
       <c r="F95" s="85"/>
       <c r="G95" s="12"/>
     </row>
-    <row r="96" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B96" s="12"/>
       <c r="C96" s="85"/>
       <c r="D96" s="85"/>
@@ -4544,7 +4565,7 @@
       <c r="F96" s="85"/>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B97" s="12"/>
       <c r="C97" s="85"/>
       <c r="D97" s="85"/>
@@ -4552,7 +4573,7 @@
       <c r="F97" s="85"/>
       <c r="G97" s="12"/>
     </row>
-    <row r="98" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B98" s="12"/>
       <c r="C98" s="85"/>
       <c r="D98" s="85"/>
@@ -4560,7 +4581,7 @@
       <c r="F98" s="85"/>
       <c r="G98" s="12"/>
     </row>
-    <row r="99" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B99" s="12"/>
       <c r="C99" s="85"/>
       <c r="D99" s="85"/>
@@ -4568,7 +4589,7 @@
       <c r="F99" s="85"/>
       <c r="G99" s="12"/>
     </row>
-    <row r="100" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B100" s="12"/>
       <c r="C100" s="85"/>
       <c r="D100" s="85"/>
@@ -4576,7 +4597,7 @@
       <c r="F100" s="85"/>
       <c r="G100" s="12"/>
     </row>
-    <row r="101" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B101" s="12"/>
       <c r="C101" s="85"/>
       <c r="D101" s="85"/>
@@ -4584,7 +4605,7 @@
       <c r="F101" s="85"/>
       <c r="G101" s="12"/>
     </row>
-    <row r="102" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B102" s="12"/>
       <c r="C102" s="86"/>
       <c r="D102" s="86"/>
@@ -4592,7 +4613,7 @@
       <c r="F102" s="86"/>
       <c r="G102" s="12"/>
     </row>
-    <row r="103" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
@@ -4600,7 +4621,7 @@
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
     </row>
-    <row r="104" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
@@ -4608,17 +4629,17 @@
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="2:7" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
       <c r="D105" s="79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E105" s="79"/>
       <c r="F105" s="79"/>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="2:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:7" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="15" t="s">
@@ -4632,7 +4653,7 @@
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="2:7" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="16" t="s">
@@ -4646,7 +4667,7 @@
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="17" t="s">
@@ -4660,7 +4681,7 @@
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="17" t="s">
@@ -4674,7 +4695,7 @@
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="17" t="s">
@@ -4688,7 +4709,7 @@
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="2:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="21" t="s">
@@ -4700,7 +4721,7 @@
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="2:7" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
@@ -4708,7 +4729,7 @@
       <c r="F112" s="47"/>
       <c r="G112" s="12"/>
     </row>
-    <row r="113" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
@@ -4716,7 +4737,7 @@
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
     </row>
-    <row r="114" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
@@ -4724,7 +4745,7 @@
       <c r="F114" s="12"/>
       <c r="G114" s="12"/>
     </row>
-    <row r="115" spans="2:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="34" t="s">
@@ -4734,7 +4755,7 @@
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
     </row>
-    <row r="116" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
@@ -4742,7 +4763,7 @@
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
     </row>
-    <row r="117" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
@@ -4768,7 +4789,7 @@
     <mergeCell ref="D25:F25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D115" location="_st2" tooltip="Step2. Lookup Table and its structure" display="Step 2."/>
+    <hyperlink ref="D115" location="_st2" tooltip="Step2. Lookup Table and its structure" display="Step 2." xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4779,27 +4800,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D68" sqref="D68:H68"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="8" collapsed="1"/>
-    <col min="3" max="3" width="7.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="55.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="8" collapsed="1"/>
+    <col min="1" max="2" width="9.109375" style="8" collapsed="1"/>
+    <col min="3" max="3" width="7.6640625" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="55.44140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.44140625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5546875" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.33203125" style="8" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.109375" style="8" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:9" s="11" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" s="11" customFormat="1" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="78" t="s">
         <v>90</v>
       </c>
@@ -4808,15 +4831,15 @@
       <c r="E3" s="78"/>
       <c r="F3" s="88"/>
     </row>
-    <row r="4" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="65"/>
       <c r="C4" s="65"/>
       <c r="D4" s="65"/>
       <c r="E4" s="65"/>
       <c r="F4" s="65"/>
     </row>
-    <row r="5" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -4826,7 +4849,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -4836,7 +4859,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="80" t="s">
         <v>48</v>
@@ -4848,7 +4871,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -4858,7 +4881,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -4868,7 +4891,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -4878,10 +4901,10 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="C12" s="84" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
@@ -4890,7 +4913,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -4900,7 +4923,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="85"/>
       <c r="D14" s="85"/>
@@ -4910,7 +4933,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="C15" s="85"/>
       <c r="D15" s="85"/>
@@ -4920,7 +4943,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="C16" s="85"/>
       <c r="D16" s="85"/>
@@ -4930,7 +4953,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="85"/>
       <c r="D17" s="85"/>
@@ -4940,7 +4963,7 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
       <c r="C18" s="85"/>
       <c r="D18" s="85"/>
@@ -4950,7 +4973,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="C19" s="85"/>
       <c r="D19" s="85"/>
@@ -4960,7 +4983,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -4970,7 +4993,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B21" s="12"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
@@ -4980,7 +5003,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -4990,7 +5013,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -5000,11 +5023,11 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="2:11" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E24" s="79"/>
       <c r="F24" s="79"/>
@@ -5012,7 +5035,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13" t="s">
@@ -5028,21 +5051,21 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13" t="s">
@@ -5056,7 +5079,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="29" t="s">
@@ -5072,7 +5095,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="17" t="s">
@@ -5088,7 +5111,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="17" t="s">
@@ -5105,7 +5128,7 @@
       <c r="I30" s="12"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="19" t="s">
@@ -5119,7 +5142,7 @@
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="2:11" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -5129,7 +5152,7 @@
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -5139,7 +5162,7 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -5149,7 +5172,7 @@
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -5159,7 +5182,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -5169,7 +5192,7 @@
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
       <c r="C37" s="87" t="s">
         <v>50</v>
@@ -5181,7 +5204,7 @@
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="67"/>
       <c r="D38" s="67"/>
@@ -5191,7 +5214,7 @@
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -5201,7 +5224,7 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="C40" s="84" t="s">
         <v>52</v>
@@ -5213,7 +5236,7 @@
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B41" s="12"/>
       <c r="C41" s="85"/>
       <c r="D41" s="85"/>
@@ -5223,7 +5246,7 @@
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
       <c r="C42" s="85"/>
       <c r="D42" s="85"/>
@@ -5233,7 +5256,7 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="86"/>
       <c r="D43" s="86"/>
@@ -5243,7 +5266,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -5253,7 +5276,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
     </row>
-    <row r="45" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -5263,11 +5286,11 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="2:9" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="79" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E46" s="79"/>
       <c r="F46" s="79"/>
@@ -5275,7 +5298,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
     </row>
-    <row r="47" spans="2:9" s="11" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" s="11" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="29" t="s">
@@ -5291,7 +5314,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
     </row>
-    <row r="48" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="17" t="s">
@@ -5307,7 +5330,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="17" t="s">
@@ -5323,7 +5346,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
     </row>
-    <row r="50" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="19" t="s">
@@ -5337,7 +5360,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -5347,7 +5370,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
     </row>
-    <row r="52" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -5357,10 +5380,10 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
       <c r="C53" s="84" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D53" s="84"/>
       <c r="E53" s="84"/>
@@ -5369,7 +5392,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="2:9" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="12"/>
       <c r="C54" s="86"/>
       <c r="D54" s="86"/>
@@ -5379,7 +5402,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
@@ -5389,7 +5412,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
     </row>
-    <row r="56" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -5399,7 +5422,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
     </row>
-    <row r="57" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
@@ -5409,7 +5432,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
     </row>
-    <row r="58" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -5419,7 +5442,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
     </row>
-    <row r="59" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
@@ -5429,7 +5452,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
     </row>
-    <row r="60" spans="2:9" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" s="11" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="12"/>
       <c r="C60" s="87" t="s">
         <v>53</v>
@@ -5441,7 +5464,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
     </row>
-    <row r="61" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -5451,7 +5474,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
     </row>
-    <row r="62" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
@@ -5461,7 +5484,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
     </row>
-    <row r="63" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B63" s="12"/>
       <c r="C63" s="84" t="s">
         <v>59</v>
@@ -5473,7 +5496,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
     </row>
-    <row r="64" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B64" s="12"/>
       <c r="C64" s="85"/>
       <c r="D64" s="85"/>
@@ -5483,7 +5506,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
     </row>
-    <row r="65" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B65" s="12"/>
       <c r="C65" s="86"/>
       <c r="D65" s="86"/>
@@ -5493,7 +5516,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
     </row>
-    <row r="66" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
@@ -5503,7 +5526,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
     </row>
-    <row r="67" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -5513,11 +5536,11 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="2:9" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="79" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E68" s="79"/>
       <c r="F68" s="79"/>
@@ -5525,11 +5548,11 @@
       <c r="H68" s="79"/>
       <c r="I68" s="12"/>
     </row>
-    <row r="69" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="89" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E69" s="94" t="s">
         <v>42</v>
@@ -5541,7 +5564,7 @@
       <c r="H69" s="94"/>
       <c r="I69" s="12"/>
     </row>
-    <row r="70" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="89"/>
@@ -5559,7 +5582,7 @@
       </c>
       <c r="I70" s="12"/>
     </row>
-    <row r="71" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="17" t="s">
@@ -5579,7 +5602,7 @@
       </c>
       <c r="I71" s="12"/>
     </row>
-    <row r="72" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="17" t="s">
@@ -5599,7 +5622,7 @@
       </c>
       <c r="I72" s="12"/>
     </row>
-    <row r="73" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="17" t="s">
@@ -5619,7 +5642,7 @@
       </c>
       <c r="I73" s="12"/>
     </row>
-    <row r="74" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="19" t="s">
@@ -5639,7 +5662,7 @@
       </c>
       <c r="I74" s="12"/>
     </row>
-    <row r="75" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
@@ -5649,7 +5672,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
     </row>
-    <row r="76" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -5659,7 +5682,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
     </row>
-    <row r="77" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -5669,7 +5692,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
     </row>
-    <row r="78" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -5679,7 +5702,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
     </row>
-    <row r="79" spans="2:9" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="34" t="s">
@@ -5691,7 +5714,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
     </row>
-    <row r="80" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -5701,7 +5724,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
     </row>
-    <row r="81" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -5731,7 +5754,7 @@
     <mergeCell ref="G69:H69"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D79" location="_st3" tooltip="Step3. Examples of Decision Tables" display="Step 3."/>
+    <hyperlink ref="D79" location="_st3" tooltip="Step3. Examples of Decision Tables" display="Step 3." xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5742,27 +5765,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -5771,7 +5794,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5780,7 +5803,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="78" t="s">
         <v>62</v>
@@ -5793,7 +5816,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -5803,7 +5826,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -5813,7 +5836,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -5825,7 +5848,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -5837,7 +5860,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="80" t="s">
         <v>63</v>
@@ -5851,7 +5874,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -5863,7 +5886,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -5875,7 +5898,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -5887,7 +5910,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="84" t="s">
         <v>64</v>
@@ -5901,7 +5924,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -5913,7 +5936,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
@@ -5925,7 +5948,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -5937,7 +5960,7 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -5949,7 +5972,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -5961,7 +5984,7 @@
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -5973,7 +5996,7 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -5985,7 +6008,7 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" s="8" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="96" t="s">
         <v>65</v>
@@ -5999,7 +6022,7 @@
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="66"/>
       <c r="D21" s="66"/>
@@ -6011,7 +6034,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -6023,10 +6046,10 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="2:11" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="79" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="79"/>
       <c r="E23" s="79"/>
@@ -6037,7 +6060,7 @@
       <c r="J23" s="79"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="13" t="s">
         <v>1</v>
@@ -6065,7 +6088,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="C25" s="13" t="s">
         <v>2</v>
@@ -6093,7 +6116,7 @@
       </c>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="C26" s="35" t="s">
         <v>13</v>
@@ -6121,13 +6144,13 @@
       </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="F27" s="69"/>
       <c r="G27" s="69"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -6139,7 +6162,7 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="84" t="s">
         <v>66</v>
@@ -6153,7 +6176,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="C30" s="85"/>
       <c r="D30" s="85"/>
@@ -6165,7 +6188,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="85"/>
       <c r="D31" s="85"/>
@@ -6177,7 +6200,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="85"/>
       <c r="D32" s="85"/>
@@ -6189,7 +6212,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="86"/>
       <c r="D33" s="86"/>
@@ -6201,7 +6224,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -6213,7 +6236,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -6225,7 +6248,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -6237,7 +6260,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -6249,7 +6272,7 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -6261,7 +6284,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="8" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="C39" s="87" t="s">
         <v>67</v>
@@ -6275,7 +6298,7 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="67"/>
       <c r="D40" s="67"/>
@@ -6287,7 +6310,7 @@
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -6299,7 +6322,7 @@
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
     </row>
-    <row r="42" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="84" t="s">
         <v>68</v>
@@ -6313,7 +6336,7 @@
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="C43" s="85"/>
       <c r="D43" s="85"/>
@@ -6325,7 +6348,7 @@
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="C44" s="85"/>
       <c r="D44" s="85"/>
@@ -6337,7 +6360,7 @@
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="C45" s="85"/>
       <c r="D45" s="85"/>
@@ -6349,7 +6372,7 @@
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="86"/>
       <c r="D46" s="86"/>
@@ -6361,7 +6384,7 @@
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -6373,7 +6396,7 @@
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -6385,11 +6408,11 @@
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E49" s="79"/>
       <c r="F49" s="79"/>
@@ -6399,7 +6422,7 @@
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
     </row>
-    <row r="50" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="95" t="s">
@@ -6415,7 +6438,7 @@
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="95" t="s">
@@ -6431,7 +6454,7 @@
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13" t="s">
@@ -6449,7 +6472,7 @@
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="31" t="s">
@@ -6467,7 +6490,7 @@
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="16">
@@ -6485,7 +6508,7 @@
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="17">
@@ -6503,7 +6526,7 @@
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="17">
@@ -6521,7 +6544,7 @@
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="19">
@@ -6539,7 +6562,7 @@
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
     </row>
-    <row r="58" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -6551,7 +6574,7 @@
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
@@ -6563,7 +6586,7 @@
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -6575,7 +6598,7 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -6587,7 +6610,7 @@
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
@@ -6599,7 +6622,7 @@
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="8" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="12"/>
       <c r="C63" s="87" t="s">
         <v>70</v>
@@ -6613,7 +6636,7 @@
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="C64" s="67"/>
       <c r="D64" s="67"/>
@@ -6625,7 +6648,7 @@
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
     </row>
-    <row r="65" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
@@ -6637,10 +6660,10 @@
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
     </row>
-    <row r="66" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
       <c r="C66" s="84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D66" s="84"/>
       <c r="E66" s="84"/>
@@ -6651,7 +6674,7 @@
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
       <c r="C67" s="85"/>
       <c r="D67" s="85"/>
@@ -6663,7 +6686,7 @@
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
       <c r="C68" s="85"/>
       <c r="D68" s="85"/>
@@ -6675,7 +6698,7 @@
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
       <c r="C69" s="85"/>
       <c r="D69" s="85"/>
@@ -6687,7 +6710,7 @@
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="C70" s="85"/>
       <c r="D70" s="85"/>
@@ -6699,7 +6722,7 @@
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
     </row>
-    <row r="71" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
       <c r="C71" s="85"/>
       <c r="D71" s="85"/>
@@ -6711,7 +6734,7 @@
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
     </row>
-    <row r="72" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="C72" s="85"/>
       <c r="D72" s="85"/>
@@ -6723,7 +6746,7 @@
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="C73" s="85"/>
       <c r="D73" s="85"/>
@@ -6735,7 +6758,7 @@
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
     </row>
-    <row r="74" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
       <c r="C74" s="85"/>
       <c r="D74" s="85"/>
@@ -6748,7 +6771,7 @@
       <c r="K74" s="12"/>
       <c r="N74" s="41"/>
     </row>
-    <row r="75" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="C75" s="86"/>
       <c r="D75" s="86"/>
@@ -6760,7 +6783,7 @@
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -6772,7 +6795,7 @@
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -6784,12 +6807,12 @@
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="2:14" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:14" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="79" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F78" s="79"/>
       <c r="G78" s="12"/>
@@ -6798,7 +6821,7 @@
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -6814,7 +6837,7 @@
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -6830,7 +6853,7 @@
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -6846,7 +6869,7 @@
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
     </row>
-    <row r="82" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
@@ -6862,7 +6885,7 @@
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -6878,7 +6901,7 @@
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
@@ -6894,7 +6917,7 @@
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
     </row>
-    <row r="85" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
@@ -6910,7 +6933,7 @@
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -6926,7 +6949,7 @@
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -6938,7 +6961,7 @@
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -6950,7 +6973,7 @@
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="89" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
       <c r="C89" s="84" t="s">
         <v>78</v>
@@ -6964,7 +6987,7 @@
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
     </row>
-    <row r="90" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
       <c r="C90" s="85"/>
       <c r="D90" s="85"/>
@@ -6976,7 +6999,7 @@
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B91" s="12"/>
       <c r="C91" s="86"/>
       <c r="D91" s="86"/>
@@ -6988,7 +7011,7 @@
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -7000,7 +7023,7 @@
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -7012,12 +7035,12 @@
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
     </row>
-    <row r="94" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
       <c r="E94" s="79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F94" s="79"/>
       <c r="G94" s="12"/>
@@ -7026,7 +7049,7 @@
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -7042,7 +7065,7 @@
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
@@ -7058,7 +7081,7 @@
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -7074,7 +7097,7 @@
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
     </row>
-    <row r="98" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -7090,7 +7113,7 @@
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
@@ -7106,7 +7129,7 @@
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -7118,7 +7141,7 @@
       <c r="J100" s="12"/>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
@@ -7130,7 +7153,7 @@
       <c r="J101" s="12"/>
       <c r="K101" s="12"/>
     </row>
-    <row r="102" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
@@ -7142,7 +7165,7 @@
       <c r="J102" s="12"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
@@ -7154,7 +7177,7 @@
       <c r="J103" s="12"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
@@ -7166,7 +7189,7 @@
       <c r="J104" s="12"/>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:11" s="8" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="12"/>
       <c r="C105" s="96" t="s">
         <v>83</v>
@@ -7180,7 +7203,7 @@
       <c r="J105" s="12"/>
       <c r="K105" s="12"/>
     </row>
-    <row r="106" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B106" s="12"/>
       <c r="C106" s="66"/>
       <c r="D106" s="66"/>
@@ -7192,7 +7215,7 @@
       <c r="J106" s="12"/>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
@@ -7204,12 +7227,12 @@
       <c r="J107" s="12"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:11" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="79" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F108" s="79"/>
       <c r="G108" s="12"/>
@@ -7218,7 +7241,7 @@
       <c r="J108" s="12"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
@@ -7234,7 +7257,7 @@
       <c r="J109" s="12"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="2:11" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:11" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
@@ -7250,7 +7273,7 @@
       <c r="J110" s="12"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
@@ -7266,7 +7289,7 @@
       <c r="J111" s="12"/>
       <c r="K111" s="12"/>
     </row>
-    <row r="112" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
@@ -7282,7 +7305,7 @@
       <c r="J112" s="12"/>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
@@ -7298,7 +7321,7 @@
       <c r="J113" s="12"/>
       <c r="K113" s="12"/>
     </row>
-    <row r="114" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
@@ -7314,7 +7337,7 @@
       <c r="J114" s="12"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="12"/>
@@ -7330,7 +7353,7 @@
       <c r="J115" s="12"/>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:11" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
@@ -7346,7 +7369,7 @@
       <c r="J116" s="12"/>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:11" s="8" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
@@ -7358,7 +7381,7 @@
       <c r="J117" s="12"/>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
       <c r="D118" s="12"/>
@@ -7370,7 +7393,7 @@
       <c r="J118" s="12"/>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B119" s="12"/>
       <c r="C119" s="97" t="s">
         <v>87</v>
@@ -7384,7 +7407,7 @@
       <c r="J119" s="12"/>
       <c r="K119" s="12"/>
     </row>
-    <row r="120" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B120" s="12"/>
       <c r="C120" s="98"/>
       <c r="D120" s="98"/>
@@ -7396,7 +7419,7 @@
       <c r="J120" s="12"/>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
       <c r="D121" s="12"/>
@@ -7408,7 +7431,7 @@
       <c r="J121" s="12"/>
       <c r="K121" s="12"/>
     </row>
-    <row r="122" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
       <c r="D122" s="12"/>
@@ -7420,10 +7443,10 @@
       <c r="J122" s="12"/>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B123" s="12"/>
       <c r="C123" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D123" s="97"/>
       <c r="E123" s="97"/>
@@ -7434,7 +7457,7 @@
       <c r="J123" s="12"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B124" s="12"/>
       <c r="C124" s="98"/>
       <c r="D124" s="98"/>
@@ -7446,7 +7469,7 @@
       <c r="J124" s="12"/>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
@@ -7458,7 +7481,7 @@
       <c r="J125" s="12"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
       <c r="D126" s="12"/>
@@ -7470,7 +7493,7 @@
       <c r="J126" s="12"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:11" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>

</xml_diff>